<commit_message>
Small fixes to terms
</commit_message>
<xml_diff>
--- a/pybron/rws_ketentest/data/BROObject - GMW data file NL samengevoegd (v2.x).xlsx
+++ b/pybron/rws_ketentest/data/BROObject - GMW data file NL samengevoegd (v2.x).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\RWS Ketentest\basis-python-project\rws_ketentest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AFC1BE5-B64C-45E6-B69E-1BE5DFC22942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8A7A79-12F0-42F6-9576-3CDCFDA51361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="4500" windowWidth="21600" windowHeight="11388" activeTab="2" xr2:uid="{26814B37-6F38-4D5A-99CF-A0A5CD7480CB}"/>
+    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" activeTab="2" xr2:uid="{26814B37-6F38-4D5A-99CF-A0A5CD7480CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Toelichting" sheetId="8" r:id="rId1"/>
@@ -133,15 +133,6 @@
     <t>[m]</t>
   </si>
   <si>
-    <t>CRS</t>
-  </si>
-  <si>
-    <t>electrodePackingMaterial</t>
-  </si>
-  <si>
-    <t>electrodeStatus</t>
-  </si>
-  <si>
     <t>BWsb</t>
   </si>
   <si>
@@ -767,6 +758,15 @@
   </si>
   <si>
     <t xml:space="preserve">Grondwatermonitoringput (GMW) </t>
+  </si>
+  <si>
+    <t>referentiestelsel</t>
+  </si>
+  <si>
+    <t>aanvulmateriaal elektrode</t>
+  </si>
+  <si>
+    <t>elektrodestatus</t>
   </si>
 </sst>
 </file>
@@ -1617,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -1633,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -1681,13 +1681,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F5" s="12"/>
       <c r="H5" s="5"/>
@@ -1699,7 +1699,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -1715,7 +1715,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1728,37 +1728,37 @@
     </row>
     <row r="9" spans="1:10" ht="23.25">
       <c r="A9" s="22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="23" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="23" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="23" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="23" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="23" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="10.15" customHeight="1">
@@ -1766,13 +1766,13 @@
     </row>
     <row r="17" spans="1:1" ht="23.25">
       <c r="A17" s="22" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="7.9" customHeight="1"/>
     <row r="33" spans="1:1" ht="23.25">
       <c r="A33" s="22" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1833,103 +1833,103 @@
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="R1" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y1" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE1" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF1" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="AG1" s="10" t="s">
         <v>179</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>169</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="N1" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="R1" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="X1" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y1" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z1" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA1" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="AB1" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="AC1" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="AD1" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="AE1" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="AF1" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="AG1" s="10" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:33">
@@ -1949,85 +1949,85 @@
         <v>11</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I2" s="37" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="N2" s="37" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="P2" s="29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="R2" s="37" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="S2" s="29" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="T2" s="29" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="U2" s="29" t="s">
         <v>15</v>
       </c>
       <c r="V2" s="29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="W2" s="29" t="s">
         <v>15</v>
       </c>
       <c r="X2" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="Y2" s="37" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="Z2" s="29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AA2" s="29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AB2" s="29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AC2" s="29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AD2" s="29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AE2" s="11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AF2" s="37" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AG2" s="11" t="s">
         <v>8</v>
@@ -2041,53 +2041,53 @@
       <c r="H3" s="39"/>
       <c r="I3" s="40"/>
       <c r="L3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M3" s="39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N3" s="40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q3" s="39" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R3" s="40"/>
       <c r="V3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="X3" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Y3" s="40" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AA3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AB3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AC3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AD3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AE3" s="39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AF3" s="40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AG3" s="39"/>
     </row>
@@ -2099,53 +2099,53 @@
       <c r="H4" s="39"/>
       <c r="I4" s="40"/>
       <c r="L4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M4" s="39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N4" s="40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q4" s="39" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R4" s="40"/>
       <c r="V4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="X4" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Y4" s="40" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AA4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AB4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AC4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AD4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AE4" s="39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AF4" s="40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AG4" s="39"/>
     </row>
@@ -2157,53 +2157,53 @@
       <c r="H5" s="39"/>
       <c r="I5" s="40"/>
       <c r="L5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M5" s="39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N5" s="40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q5" s="39" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R5" s="40"/>
       <c r="V5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="X5" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Y5" s="40" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AA5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AB5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AC5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AD5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AE5" s="39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AF5" s="40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AG5" s="39"/>
     </row>
@@ -2215,53 +2215,53 @@
       <c r="H6" s="39"/>
       <c r="I6" s="40"/>
       <c r="L6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M6" s="39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N6" s="40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q6" s="39" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R6" s="40"/>
       <c r="V6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="X6" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Y6" s="40" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AA6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AB6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AC6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AD6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AE6" s="39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AF6" s="40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AG6" s="39"/>
     </row>
@@ -2273,53 +2273,53 @@
       <c r="H7" s="39"/>
       <c r="I7" s="40"/>
       <c r="L7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M7" s="39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N7" s="40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q7" s="39" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R7" s="40"/>
       <c r="V7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="X7" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Y7" s="40" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AA7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AB7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AC7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AD7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AE7" s="39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AF7" s="40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AG7" s="39"/>
     </row>
@@ -2331,53 +2331,53 @@
       <c r="H8" s="39"/>
       <c r="I8" s="40"/>
       <c r="L8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M8" s="39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N8" s="40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q8" s="39" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R8" s="40"/>
       <c r="V8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="X8" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Y8" s="40" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AA8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AB8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AC8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AD8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AE8" s="39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AF8" s="40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AG8" s="39"/>
     </row>
@@ -2389,53 +2389,53 @@
       <c r="H9" s="39"/>
       <c r="I9" s="40"/>
       <c r="L9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M9" s="39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N9" s="40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q9" s="39" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R9" s="40"/>
       <c r="V9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="X9" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Y9" s="40" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AA9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AB9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AC9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AD9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AE9" s="39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AF9" s="40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AG9" s="39"/>
     </row>
@@ -2447,53 +2447,53 @@
       <c r="H10" s="39"/>
       <c r="I10" s="40"/>
       <c r="L10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M10" s="39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N10" s="40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q10" s="39" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R10" s="40"/>
       <c r="V10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="X10" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Y10" s="40" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AA10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AB10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AC10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AD10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AE10" s="39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AF10" s="40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AG10" s="39"/>
     </row>
@@ -2510,57 +2510,57 @@
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M11" s="35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N11" s="25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O11" s="15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P11" s="15" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q11" s="35" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R11" s="25"/>
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
       <c r="V11" s="15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="W11" s="15"/>
       <c r="X11" s="35" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Y11" s="25" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z11" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AA11" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AB11" s="15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AC11" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AD11" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AE11" s="35" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AF11" s="25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AG11" s="35"/>
     </row>
@@ -2673,8 +2673,8 @@
   </sheetPr>
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2701,551 +2701,551 @@
   <sheetData>
     <row r="1" spans="1:18" s="15" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D1" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>126</v>
-      </c>
       <c r="I1" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="N1" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q1" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="O1" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" s="36" t="s">
-        <v>138</v>
-      </c>
       <c r="R1" s="36" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
         <v>60</v>
       </c>
-      <c r="I2" t="s">
-        <v>63</v>
-      </c>
       <c r="J2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
         <v>67</v>
       </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" t="s">
-        <v>74</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" t="s">
-        <v>70</v>
-      </c>
       <c r="P2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Q2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="R2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" t="s">
         <v>61</v>
       </c>
-      <c r="I3" t="s">
-        <v>64</v>
-      </c>
       <c r="J3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="N3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="O3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="P3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="Q3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="R3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" t="s">
         <v>62</v>
       </c>
-      <c r="I4" t="s">
-        <v>65</v>
-      </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="O4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="R4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="N5" s="26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="Q5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Q6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="Q8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="26" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="B11" s="26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="E12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" t="s">
         <v>43</v>
       </c>
-      <c r="J12" t="s">
-        <v>46</v>
-      </c>
       <c r="M12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="E13" s="26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" t="s">
         <v>44</v>
       </c>
-      <c r="J13" t="s">
-        <v>47</v>
-      </c>
       <c r="M13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Q13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="E14" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="J14" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="G14" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="J14" s="26" t="s">
-        <v>158</v>
-      </c>
       <c r="M14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="Q14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="E15" s="26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="Q15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="E16" s="26" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="Q16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="E17" s="26" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J17" s="26" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M17" s="26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="J18" s="26" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="M18" s="26" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="M19" s="26" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="M20" s="26" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="M21" s="26" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="23" spans="1:13" ht="15.75" thickBot="1">
       <c r="A23" s="27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B23" s="28"/>
     </row>

</xml_diff>